<commit_message>
Update device to module mapping.
</commit_message>
<xml_diff>
--- a/docs/device_to_module_mapping.xlsx
+++ b/docs/device_to_module_mapping.xlsx
@@ -87,10 +87,10 @@
     <t>LS2085a Rev1 API</t>
   </si>
   <si>
-    <t>LS1088a Rev1 Implementation</t>
-  </si>
-  <si>
-    <t>LS1088a Rev1 API</t>
+    <t>LS1088a Rev1 + LS2088a Rev1 API</t>
+  </si>
+  <si>
+    <t>LS1088a Rev1 + LS2088a Rev1 Implementation</t>
   </si>
 </sst>
 </file>
@@ -516,7 +516,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -524,8 +524,8 @@
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -539,10 +539,10 @@
         <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5">

</xml_diff>